<commit_message>
Updated transcation file in 27.04.2017
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23835" windowHeight="9810"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23835" windowHeight="7605"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="125">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -443,10 +443,6 @@
     <t xml:space="preserve">        -----</t>
   </si>
   <si>
-    <t xml:space="preserve">
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">            0.0255USDT</t>
   </si>
   <si>
@@ -491,6 +487,45 @@
   </si>
   <si>
     <t xml:space="preserve">            0.0362USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            77.5USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-04-27 09:40:37  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-04-26 18:59:06
+</t>
+  </si>
+  <si>
+    <t>0.00974957 USDT (0.15%)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ~1.5%</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">4/27/2017  9:40:37 AM
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           0.0285USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          435 NXT</t>
   </si>
 </sst>
 </file>
@@ -931,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG27"/>
+  <dimension ref="A1:DG29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,10 +1855,10 @@
         <v>91</v>
       </c>
       <c r="H24" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1840,19 +1875,19 @@
         <v>2.896926E-2</v>
       </c>
       <c r="E25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" t="s">
         <v>107</v>
-      </c>
-      <c r="F25" t="s">
-        <v>108</v>
       </c>
       <c r="G25" t="s">
         <v>95</v>
       </c>
       <c r="H25" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1863,28 +1898,28 @@
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D26">
         <v>3.5388879999999998E-2</v>
       </c>
       <c r="E26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26" t="s">
+        <v>109</v>
+      </c>
+      <c r="G26" t="s">
         <v>111</v>
-      </c>
-      <c r="F26" t="s">
-        <v>110</v>
-      </c>
-      <c r="G26" t="s">
-        <v>112</v>
       </c>
       <c r="H26" t="s">
         <v>45</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1892,29 +1927,94 @@
         <v>42851.395914351851</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D27">
         <v>3.5388879999999998E-2</v>
       </c>
       <c r="E27" t="s">
+        <v>116</v>
+      </c>
+      <c r="F27" t="s">
+        <v>115</v>
+      </c>
+      <c r="G27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="J27" t="s">
+        <v>120</v>
+      </c>
+      <c r="K27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>42852.40320601852</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28">
+        <v>78.770000580000001</v>
+      </c>
+      <c r="E28" t="s">
         <v>117</v>
       </c>
-      <c r="F27" t="s">
-        <v>116</v>
-      </c>
-      <c r="G27" t="s">
-        <v>112</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="F28" t="s">
+        <v>93</v>
+      </c>
+      <c r="G28" t="s">
+        <v>91</v>
+      </c>
+      <c r="H28" t="s">
         <v>86</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>106</v>
-      </c>
+      <c r="I28" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>42852.40320601852</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29">
+        <v>2.896926E-2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>123</v>
+      </c>
+      <c r="F29" t="s">
+        <v>124</v>
+      </c>
+      <c r="G29" t="s">
+        <v>95</v>
+      </c>
+      <c r="H29" t="s">
+        <v>86</v>
+      </c>
+      <c r="I29" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated file in 15 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="138">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -380,10 +380,6 @@
     <t xml:space="preserve">            73.6USDT</t>
   </si>
   <si>
-    <t xml:space="preserve"> 
-</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ZEC/USDT0000003</t>
   </si>
   <si>
@@ -550,6 +546,39 @@
   </si>
   <si>
     <t xml:space="preserve">           0.030USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-04-27 19:26:55 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ETH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ETH/USDT0000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.13 ETH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          63.998USDT</t>
+  </si>
+  <si>
+    <t>0.00019500 ETH (0.15%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    63.88301000
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  63.88301000
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          66USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.1298 ETH</t>
   </si>
 </sst>
 </file>
@@ -647,7 +676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -655,6 +684,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -990,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG30"/>
+  <dimension ref="A1:DG32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,7 +1754,7 @@
         <v>88</v>
       </c>
       <c r="L19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1754,10 +1786,10 @@
         <v>42851.803194444445</v>
       </c>
       <c r="K20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1789,13 +1821,13 @@
         <v>42847.803194444445</v>
       </c>
       <c r="J21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K21" t="s">
         <v>98</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>99</v>
-      </c>
-      <c r="L21" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1812,19 +1844,19 @@
         <v>71.489997959999997</v>
       </c>
       <c r="E22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" t="s">
         <v>92</v>
       </c>
-      <c r="F22" t="s">
-        <v>93</v>
-      </c>
       <c r="G22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H22" t="s">
         <v>60</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1835,25 +1867,25 @@
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D23">
         <v>2.1299999999999999E-2</v>
       </c>
       <c r="E23" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" t="s">
         <v>96</v>
       </c>
-      <c r="F23" t="s">
-        <v>97</v>
-      </c>
       <c r="G23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H23" t="s">
         <v>60</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1870,19 +1902,19 @@
         <v>79.232641130000005</v>
       </c>
       <c r="E24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H24" t="s">
         <v>60</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1893,25 +1925,25 @@
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D25">
         <v>2.896926E-2</v>
       </c>
       <c r="E25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" t="s">
         <v>106</v>
       </c>
-      <c r="F25" t="s">
-        <v>107</v>
-      </c>
       <c r="G25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H25" t="s">
         <v>60</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1922,28 +1954,28 @@
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D26">
         <v>3.5388879999999998E-2</v>
       </c>
       <c r="E26" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" t="s">
         <v>110</v>
-      </c>
-      <c r="F26" t="s">
-        <v>109</v>
-      </c>
-      <c r="G26" t="s">
-        <v>111</v>
       </c>
       <c r="H26" t="s">
         <v>45</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1951,34 +1983,34 @@
         <v>42851.395914351851</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D27">
         <v>3.5388879999999998E-2</v>
       </c>
       <c r="E27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H27" t="s">
         <v>45</v>
       </c>
       <c r="I27" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="J27" t="s">
         <v>119</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>120</v>
-      </c>
-      <c r="K27" t="s">
-        <v>121</v>
       </c>
       <c r="L27" t="s">
         <v>81</v>
@@ -1998,19 +2030,19 @@
         <v>78.770000580000001</v>
       </c>
       <c r="E28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H28" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2021,19 +2053,19 @@
         <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D29">
         <v>2.896926E-2</v>
       </c>
       <c r="E29" t="s">
+        <v>122</v>
+      </c>
+      <c r="F29" t="s">
         <v>123</v>
       </c>
-      <c r="F29" t="s">
-        <v>124</v>
-      </c>
       <c r="G29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H29" t="s">
         <v>45</v>
@@ -2042,7 +2074,7 @@
         <v>42852.556944444441</v>
       </c>
       <c r="J29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2050,27 +2082,86 @@
         <v>42852.556944444441</v>
       </c>
       <c r="B30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D30">
         <v>2.8400000000000002E-2</v>
       </c>
       <c r="E30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H30" t="s">
         <v>86</v>
       </c>
       <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>42852.556944444441</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" t="s">
+        <v>132</v>
+      </c>
+      <c r="F31" t="s">
+        <v>131</v>
+      </c>
+      <c r="G31" t="s">
+        <v>130</v>
+      </c>
+      <c r="H31" t="s">
+        <v>45</v>
+      </c>
+      <c r="I31" s="6">
+        <v>42852.556944444441</v>
+      </c>
+      <c r="J31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>42852.556944444441</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E32" t="s">
+        <v>136</v>
+      </c>
+      <c r="F32" t="s">
+        <v>137</v>
+      </c>
+      <c r="G32" t="s">
+        <v>130</v>
+      </c>
+      <c r="H32" t="s">
+        <v>86</v>
+      </c>
+      <c r="I32" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated file at 28.04.2017 in 30 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="149">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -579,6 +579,64 @@
   </si>
   <si>
     <t xml:space="preserve">         0.1298 ETH</t>
+  </si>
+  <si>
+    <t>0.01954564 USDT (0.15%)</t>
+  </si>
+  <si>
+    <t>0.01285070 USDT (0.15%)</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>~4.9%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>~2.8%</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">        0.347 ETH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ETH/USDT0000002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          63.5USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 68.01353473
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              1420USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0.00078869 BTC</t>
   </si>
 </sst>
 </file>
@@ -1022,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG32"/>
+  <dimension ref="A1:DG34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2100,9 +2158,20 @@
         <v>94</v>
       </c>
       <c r="H30" t="s">
-        <v>86</v>
-      </c>
-      <c r="I30" s="6"/>
+        <v>45</v>
+      </c>
+      <c r="I30" s="6">
+        <v>42853.36923611111</v>
+      </c>
+      <c r="J30" t="s">
+        <v>138</v>
+      </c>
+      <c r="K30" t="s">
+        <v>141</v>
+      </c>
+      <c r="L30" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
@@ -2159,9 +2228,74 @@
         <v>130</v>
       </c>
       <c r="H32" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" s="6">
+        <v>42852.866249999999</v>
+      </c>
+      <c r="J32" t="s">
+        <v>139</v>
+      </c>
+      <c r="K32" t="s">
+        <v>142</v>
+      </c>
+      <c r="L32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>42853.587916666664</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" t="s">
+        <v>145</v>
+      </c>
+      <c r="F33" t="s">
+        <v>143</v>
+      </c>
+      <c r="G33" t="s">
+        <v>144</v>
+      </c>
+      <c r="H33" t="s">
         <v>86</v>
       </c>
-      <c r="I32" s="6"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>42853.589432870373</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>1382.89918891</v>
+      </c>
+      <c r="E34" t="s">
+        <v>147</v>
+      </c>
+      <c r="F34" t="s">
+        <v>148</v>
+      </c>
+      <c r="G34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H34" t="s">
+        <v>86</v>
+      </c>
+      <c r="I34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated file at 02.05.2017 in 20 min.
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="159">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -647,6 +647,28 @@
   </si>
   <si>
     <t xml:space="preserve">        0.340 ETH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2017-05-02 13:41:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          6.66USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        3.4ETC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 6.80
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              1600USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     0.00061456 BTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00167991 USDT (0.15%) </t>
   </si>
 </sst>
 </file>
@@ -1090,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG35"/>
+  <dimension ref="A1:DG37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,7 +2275,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>42853.587916666664</v>
       </c>
@@ -2282,7 +2304,7 @@
         <v>42853.843217592592</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>42853.589432870373</v>
       </c>
@@ -2305,11 +2327,16 @@
         <v>40</v>
       </c>
       <c r="H34" t="s">
-        <v>86</v>
-      </c>
-      <c r="I34" s="4"/>
-    </row>
-    <row r="35" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="I34" s="4">
+        <v>42853.984583333331</v>
+      </c>
+      <c r="J34" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>42853.843217592592</v>
       </c>
@@ -2332,9 +2359,65 @@
         <v>144</v>
       </c>
       <c r="H35" t="s">
+        <v>60</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>42857.570335648146</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E36" t="s">
+        <v>153</v>
+      </c>
+      <c r="F36" t="s">
+        <v>154</v>
+      </c>
+      <c r="G36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" t="s">
         <v>86</v>
       </c>
-      <c r="I35" s="6"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>42857.730462962965</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37">
+        <v>1571</v>
+      </c>
+      <c r="E37" t="s">
+        <v>156</v>
+      </c>
+      <c r="F37" t="s">
+        <v>157</v>
+      </c>
+      <c r="G37" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" t="s">
+        <v>86</v>
+      </c>
+      <c r="I37" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated at 03.05.2017 in 15 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="162">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -669,6 +669,16 @@
   </si>
   <si>
     <t xml:space="preserve">0.00167991 USDT (0.15%) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">          6.9USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        3.3ETC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 7.09000022
+</t>
   </si>
 </sst>
 </file>
@@ -1112,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG37"/>
+  <dimension ref="A1:DG38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2388,9 +2398,11 @@
         <v>55</v>
       </c>
       <c r="H36" t="s">
-        <v>86</v>
-      </c>
-      <c r="I36" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="I36" s="6">
+        <v>42858.524247685185</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
@@ -2418,6 +2430,33 @@
         <v>86</v>
       </c>
       <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>42858.524247685185</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E38" t="s">
+        <v>159</v>
+      </c>
+      <c r="F38" t="s">
+        <v>160</v>
+      </c>
+      <c r="G38" t="s">
+        <v>55</v>
+      </c>
+      <c r="H38" t="s">
+        <v>86</v>
+      </c>
+      <c r="I38" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated file at 05.04.2017 in 15 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="165">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -678,6 +678,16 @@
   </si>
   <si>
     <t xml:space="preserve">                 7.09000022
+</t>
+  </si>
+  <si>
+    <t>0.00147494 USDT (0.15%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          7.1USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                7.64000000
 </t>
   </si>
 </sst>
@@ -1122,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG38"/>
+  <dimension ref="A1:DG39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2427,9 +2437,14 @@
         <v>40</v>
       </c>
       <c r="H37" t="s">
-        <v>86</v>
-      </c>
-      <c r="I37" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="I37" s="4">
+        <v>42858.746388888889</v>
+      </c>
+      <c r="J37" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
@@ -2454,9 +2469,38 @@
         <v>55</v>
       </c>
       <c r="H38" t="s">
+        <v>60</v>
+      </c>
+      <c r="I38" s="6">
+        <v>42859.441886574074</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>42859.441886574074</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E39" t="s">
+        <v>163</v>
+      </c>
+      <c r="F39" t="s">
+        <v>154</v>
+      </c>
+      <c r="G39" t="s">
+        <v>55</v>
+      </c>
+      <c r="H39" t="s">
         <v>86</v>
       </c>
-      <c r="I38" s="6"/>
+      <c r="I39" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated file at 05.05.2017 in 15 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="168">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -689,6 +689,16 @@
   <si>
     <t xml:space="preserve">                7.64000000
 </t>
+  </si>
+  <si>
+    <t>0.00510000 ETC (0.15%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               7.50999943
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          7.7USDT</t>
   </si>
 </sst>
 </file>
@@ -1132,10 +1142,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG39"/>
+  <dimension ref="A1:DG40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2498,9 +2508,41 @@
         <v>55</v>
       </c>
       <c r="H39" t="s">
+        <v>45</v>
+      </c>
+      <c r="I39" s="6">
+        <v>42859.875844907408</v>
+      </c>
+      <c r="J39" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>42860.441886574074</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E40" t="s">
+        <v>167</v>
+      </c>
+      <c r="F40" t="s">
+        <v>154</v>
+      </c>
+      <c r="G40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H40" t="s">
         <v>86</v>
       </c>
-      <c r="I39" s="6"/>
+      <c r="I40" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated in 15 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="176">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -699,6 +699,43 @@
   </si>
   <si>
     <t xml:space="preserve">          7.7USDT</t>
+  </si>
+  <si>
+    <t>0.03921110 USDT (0.15%)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>~8%</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4 day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">              0.10359450
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XRP/USDT0000002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         320 XRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.085USDT</t>
   </si>
 </sst>
 </file>
@@ -1142,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG40"/>
+  <dimension ref="A1:DG41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,7 +2342,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>42853.587916666664</v>
       </c>
@@ -2334,7 +2371,7 @@
         <v>42853.843217592592</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>42853.589432870373</v>
       </c>
@@ -2366,7 +2403,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>42853.843217592592</v>
       </c>
@@ -2395,7 +2432,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>42857.570335648146</v>
       </c>
@@ -2424,7 +2461,7 @@
         <v>42858.524247685185</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>42857.730462962965</v>
       </c>
@@ -2456,7 +2493,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>42858.524247685185</v>
       </c>
@@ -2485,7 +2522,7 @@
         <v>42859.441886574074</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>42859.441886574074</v>
       </c>
@@ -2517,7 +2554,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>42860.441886574074</v>
       </c>
@@ -2540,9 +2577,50 @@
         <v>55</v>
       </c>
       <c r="H40" t="s">
+        <v>45</v>
+      </c>
+      <c r="I40" s="6">
+        <v>42860.578460648147</v>
+      </c>
+      <c r="J40" t="s">
+        <v>168</v>
+      </c>
+      <c r="K40" t="s">
+        <v>169</v>
+      </c>
+      <c r="L40" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>42860.441886574074</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E41" t="s">
+        <v>175</v>
+      </c>
+      <c r="F41" t="s">
+        <v>174</v>
+      </c>
+      <c r="G41" t="s">
+        <v>173</v>
+      </c>
+      <c r="H41" t="s">
         <v>86</v>
       </c>
-      <c r="I40" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="K41" t="s">
+        <v>171</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated at 06.05.2017 in 15 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="187">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -774,6 +774,16 @@
   <si>
     <t xml:space="preserve">              0.09750980
 </t>
+  </si>
+  <si>
+    <t>0.56250000 XRP (0.15%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              0.09535348
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.107USDT</t>
   </si>
 </sst>
 </file>
@@ -1217,10 +1227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG43"/>
+  <dimension ref="A1:DG44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2726,10 +2736,45 @@
         <v>181</v>
       </c>
       <c r="H43" t="s">
+        <v>45</v>
+      </c>
+      <c r="I43" s="6">
+        <v>42860.867835648147</v>
+      </c>
+      <c r="J43" t="s">
+        <v>184</v>
+      </c>
+      <c r="K43" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>42861.347037037034</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="E44" t="s">
+        <v>186</v>
+      </c>
+      <c r="F44" t="s">
+        <v>182</v>
+      </c>
+      <c r="G44" t="s">
+        <v>181</v>
+      </c>
+      <c r="H44" t="s">
         <v>86</v>
       </c>
-      <c r="I43" s="6"/>
-      <c r="K43" t="s">
+      <c r="I44" s="6"/>
+      <c r="K44" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated in 13 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="192">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -783,7 +783,35 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">          0.107USDT</t>
+    <t xml:space="preserve">         0.1024USDT</t>
+  </si>
+  <si>
+    <t>0.09585608 USDT (0.25%)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   ~20%</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.087USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         440 XRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              0.10170785
+</t>
   </si>
 </sst>
 </file>
@@ -1227,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG44"/>
+  <dimension ref="A1:DG45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2771,10 +2799,48 @@
         <v>181</v>
       </c>
       <c r="H44" t="s">
+        <v>45</v>
+      </c>
+      <c r="I44" s="6">
+        <v>42861.715277777781</v>
+      </c>
+      <c r="J44" t="s">
+        <v>187</v>
+      </c>
+      <c r="K44" t="s">
+        <v>188</v>
+      </c>
+      <c r="L44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>42861.715277777781</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E45" t="s">
+        <v>189</v>
+      </c>
+      <c r="F45" t="s">
+        <v>190</v>
+      </c>
+      <c r="G45" t="s">
+        <v>181</v>
+      </c>
+      <c r="H45" t="s">
         <v>86</v>
       </c>
-      <c r="I44" s="6"/>
-      <c r="K44" t="s">
+      <c r="I45" s="6"/>
+      <c r="K45" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated at 07.05.2017 in 20 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="196">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -812,6 +812,19 @@
   <si>
     <t xml:space="preserve">              0.10170785
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.096USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XRP/USDT0000004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             0.10560001
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         410 XRP</t>
   </si>
 </sst>
 </file>
@@ -1255,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG45"/>
+  <dimension ref="A1:DG46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2834,13 +2847,45 @@
         <v>190</v>
       </c>
       <c r="G45" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="H45" t="s">
+        <v>60</v>
+      </c>
+      <c r="I45" s="6">
+        <v>42862.298773148148</v>
+      </c>
+      <c r="K45" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>42862.298773148148</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E46" t="s">
+        <v>192</v>
+      </c>
+      <c r="F46" t="s">
+        <v>195</v>
+      </c>
+      <c r="G46" t="s">
+        <v>193</v>
+      </c>
+      <c r="H46" t="s">
         <v>86</v>
       </c>
-      <c r="I45" s="6"/>
-      <c r="K45" t="s">
+      <c r="I46" s="6"/>
+      <c r="K46" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated file at 08.05.2017 in 20 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="199">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -825,6 +825,16 @@
   </si>
   <si>
     <t xml:space="preserve">         410 XRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         210 XRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.185USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             0.1926
+</t>
   </si>
 </sst>
 </file>
@@ -1268,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG46"/>
+  <dimension ref="A1:DG47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2882,10 +2892,42 @@
         <v>193</v>
       </c>
       <c r="H46" t="s">
+        <v>60</v>
+      </c>
+      <c r="I46" s="6">
+        <v>42863.284270833334</v>
+      </c>
+      <c r="K46" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>42863.284270833334</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>107</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="E47" t="s">
+        <v>197</v>
+      </c>
+      <c r="F47" t="s">
+        <v>196</v>
+      </c>
+      <c r="G47" t="s">
+        <v>193</v>
+      </c>
+      <c r="H47" t="s">
         <v>86</v>
       </c>
-      <c r="I46" s="6"/>
-      <c r="K46" t="s">
+      <c r="I47" s="6"/>
+      <c r="K47" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated in 10 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="203">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -835,6 +835,19 @@
   <si>
     <t xml:space="preserve">             0.1926
 </t>
+  </si>
+  <si>
+    <t>0.31500000 XRP (0.15%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           0.18590000
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.197USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         209 XRP</t>
   </si>
 </sst>
 </file>
@@ -1278,10 +1291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG47"/>
+  <dimension ref="A1:DG48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2924,10 +2937,45 @@
         <v>193</v>
       </c>
       <c r="H47" t="s">
+        <v>45</v>
+      </c>
+      <c r="I47" s="6">
+        <v>42863.315740740742</v>
+      </c>
+      <c r="J47" t="s">
+        <v>199</v>
+      </c>
+      <c r="K47" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>42863.375740740739</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E48" t="s">
+        <v>201</v>
+      </c>
+      <c r="F48" t="s">
+        <v>202</v>
+      </c>
+      <c r="G48" t="s">
+        <v>193</v>
+      </c>
+      <c r="H48" t="s">
         <v>86</v>
       </c>
-      <c r="I47" s="6"/>
-      <c r="K47" t="s">
+      <c r="I48" s="6"/>
+      <c r="K48" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated at 10.05.2017 in 20 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23835" windowHeight="7605"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23835" windowHeight="7605"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="223">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -911,6 +911,31 @@
   </si>
   <si>
     <t xml:space="preserve">          0.03113426
+</t>
+  </si>
+  <si>
+    <t>0.03882735 USDT (0.15%)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   ~-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>35%</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.165USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        0.184
 </t>
   </si>
 </sst>
@@ -1009,7 +1034,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1022,6 +1047,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1355,10 +1382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG52"/>
+  <dimension ref="A1:DG53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,7 +1397,7 @@
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="9" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="22.5703125" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" customWidth="1"/>
@@ -1399,7 +1426,7 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -1536,7 +1563,7 @@
       <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I2" s="2">
@@ -1568,7 +1595,7 @@
       <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="2">
@@ -1600,7 +1627,7 @@
       <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="9" t="s">
         <v>35</v>
       </c>
       <c r="I4" s="4">
@@ -1629,7 +1656,7 @@
       <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I5" s="2">
@@ -1667,7 +1694,7 @@
       <c r="G6" t="s">
         <v>32</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="9" t="s">
         <v>35</v>
       </c>
       <c r="I6" s="4">
@@ -1696,7 +1723,7 @@
       <c r="G7" t="s">
         <v>21</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I7" s="2">
@@ -1728,7 +1755,7 @@
       <c r="G8" t="s">
         <v>39</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="5" t="s">
@@ -1760,7 +1787,7 @@
       <c r="G9" t="s">
         <v>40</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="4">
@@ -1792,7 +1819,7 @@
       <c r="G10" t="s">
         <v>50</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I10" s="2">
@@ -1824,7 +1851,7 @@
       <c r="G11" t="s">
         <v>54</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="9" t="s">
         <v>35</v>
       </c>
       <c r="I11" s="2">
@@ -1853,7 +1880,7 @@
       <c r="G12" t="s">
         <v>55</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="9" t="s">
         <v>35</v>
       </c>
       <c r="I12" s="2">
@@ -1882,7 +1909,7 @@
       <c r="G13" t="s">
         <v>54</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I13" s="2">
@@ -1911,7 +1938,7 @@
       <c r="G14" t="s">
         <v>50</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I14" s="2">
@@ -1949,7 +1976,7 @@
       <c r="G15" t="s">
         <v>63</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I15" s="6" t="s">
@@ -1978,7 +2005,7 @@
       <c r="G16" t="s">
         <v>63</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="9" t="s">
         <v>35</v>
       </c>
       <c r="I16" s="6">
@@ -2007,7 +2034,7 @@
       <c r="G17" t="s">
         <v>54</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I17" s="2">
@@ -2045,7 +2072,7 @@
       <c r="G18" t="s">
         <v>77</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I18" s="6" t="s">
@@ -2074,7 +2101,7 @@
       <c r="G19" t="s">
         <v>77</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I19" s="6">
@@ -2112,7 +2139,7 @@
       <c r="G20" t="s">
         <v>85</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I20" s="2">
@@ -2147,7 +2174,7 @@
       <c r="G21" t="s">
         <v>63</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="6">
@@ -2185,7 +2212,7 @@
       <c r="G22" t="s">
         <v>90</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I22" s="6" t="s">
@@ -2214,7 +2241,7 @@
       <c r="G23" t="s">
         <v>94</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I23" s="6" t="s">
@@ -2243,7 +2270,7 @@
       <c r="G24" t="s">
         <v>90</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I24" s="6" t="s">
@@ -2272,7 +2299,7 @@
       <c r="G25" t="s">
         <v>94</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I25" s="6" t="s">
@@ -2301,7 +2328,7 @@
       <c r="G26" t="s">
         <v>110</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I26" s="6" t="s">
@@ -2333,7 +2360,7 @@
       <c r="G27" t="s">
         <v>110</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I27" s="6" t="s">
@@ -2371,7 +2398,7 @@
       <c r="G28" t="s">
         <v>90</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="6" t="s">
@@ -2400,7 +2427,7 @@
       <c r="G29" t="s">
         <v>94</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I29" s="6">
@@ -2432,7 +2459,7 @@
       <c r="G30" t="s">
         <v>94</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I30" s="6">
@@ -2470,7 +2497,7 @@
       <c r="G31" t="s">
         <v>130</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I31" s="6">
@@ -2502,7 +2529,7 @@
       <c r="G32" t="s">
         <v>130</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I32" s="6">
@@ -2540,7 +2567,7 @@
       <c r="G33" t="s">
         <v>144</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I33" s="6">
@@ -2569,7 +2596,7 @@
       <c r="G34" t="s">
         <v>40</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I34" s="4">
@@ -2601,7 +2628,7 @@
       <c r="G35" t="s">
         <v>144</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I35" s="6" t="s">
@@ -2630,7 +2657,7 @@
       <c r="G36" t="s">
         <v>55</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I36" s="6">
@@ -2659,7 +2686,7 @@
       <c r="G37" t="s">
         <v>40</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I37" s="4">
@@ -2691,7 +2718,7 @@
       <c r="G38" t="s">
         <v>55</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I38" s="6">
@@ -2720,7 +2747,7 @@
       <c r="G39" t="s">
         <v>55</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I39" s="6">
@@ -2752,7 +2779,7 @@
       <c r="G40" t="s">
         <v>55</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I40" s="6">
@@ -2790,7 +2817,7 @@
       <c r="G41" t="s">
         <v>173</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I41" s="6">
@@ -2825,7 +2852,7 @@
       <c r="G42" t="s">
         <v>173</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I42" s="6">
@@ -2863,7 +2890,7 @@
       <c r="G43" t="s">
         <v>181</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I43" s="6">
@@ -2898,7 +2925,7 @@
       <c r="G44" t="s">
         <v>181</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I44" s="6">
@@ -2936,7 +2963,7 @@
       <c r="G45" t="s">
         <v>193</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I45" s="6">
@@ -2968,7 +2995,7 @@
       <c r="G46" t="s">
         <v>193</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I46" s="6">
@@ -3000,7 +3027,7 @@
       <c r="G47" t="s">
         <v>193</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I47" s="6">
@@ -3035,7 +3062,7 @@
       <c r="G48" t="s">
         <v>193</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H48" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I48" s="6">
@@ -3051,7 +3078,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>42863.398599537039</v>
       </c>
@@ -3073,7 +3100,7 @@
       <c r="G49" t="s">
         <v>205</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I49" s="6">
@@ -3083,7 +3110,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>42863.563043981485</v>
       </c>
@@ -3105,7 +3132,7 @@
       <c r="G50" t="s">
         <v>210</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H50" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I50" s="6">
@@ -3118,7 +3145,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>42863.686921296299</v>
       </c>
@@ -3140,7 +3167,7 @@
       <c r="G51" t="s">
         <v>210</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I51" s="6">
@@ -3150,7 +3177,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>42864.811342592591</v>
       </c>
@@ -3172,11 +3199,49 @@
       <c r="G52" t="s">
         <v>210</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H52" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I52" s="6">
+        <v>42864.821932870371</v>
+      </c>
+      <c r="J52" t="s">
+        <v>219</v>
+      </c>
+      <c r="K52" t="s">
+        <v>220</v>
+      </c>
+      <c r="L52" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>42865.342280092591</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s">
+        <v>107</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E53" t="s">
+        <v>221</v>
+      </c>
+      <c r="F53" t="s">
+        <v>108</v>
+      </c>
+      <c r="G53" t="s">
+        <v>205</v>
+      </c>
+      <c r="H53" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I52" s="6"/>
-      <c r="K52" t="s">
+      <c r="I53" s="6"/>
+      <c r="K53" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated file at 11.05.2017 in 20 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="236">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -971,6 +971,13 @@
   </si>
   <si>
     <t>NXT</t>
+  </si>
+  <si>
+    <t>0.26918413 XRP (0.15%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.17838400
+</t>
   </si>
 </sst>
 </file>
@@ -1416,10 +1423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG53"/>
+  <dimension ref="A1:DG54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3272,10 +3279,45 @@
         <v>205</v>
       </c>
       <c r="H53" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I53" s="6">
+        <v>42866.194872685184</v>
+      </c>
+      <c r="J53" t="s">
+        <v>234</v>
+      </c>
+      <c r="K53" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>42866.28197916667</v>
+      </c>
+      <c r="B54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="E54" t="s">
+        <v>197</v>
+      </c>
+      <c r="F54" t="s">
+        <v>108</v>
+      </c>
+      <c r="G54" t="s">
+        <v>205</v>
+      </c>
+      <c r="H54" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I53" s="6"/>
-      <c r="K53" t="s">
+      <c r="I54" s="6"/>
+      <c r="K54" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update file at 12.05.2017 in 20 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="242">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -978,6 +978,25 @@
   <si>
     <t xml:space="preserve"> 0.17838400
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04987508 USDT (0.15%) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     ~11%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        0.192
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.175USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         189 XRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XRP/USDT0000006</t>
   </si>
 </sst>
 </file>
@@ -1423,9 +1442,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG54"/>
+  <dimension ref="A1:DG55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
@@ -3314,10 +3333,48 @@
         <v>205</v>
       </c>
       <c r="H54" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I54" s="6">
+        <v>42866.613298611112</v>
+      </c>
+      <c r="J54" t="s">
+        <v>236</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="L54" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>42867.279143518521</v>
+      </c>
+      <c r="B55" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E55" t="s">
+        <v>239</v>
+      </c>
+      <c r="F55" t="s">
+        <v>240</v>
+      </c>
+      <c r="G55" t="s">
+        <v>241</v>
+      </c>
+      <c r="H55" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I54" s="6"/>
-      <c r="K54" t="s">
+      <c r="I55" s="6"/>
+      <c r="K55" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated file at 16.05.2017 in 15
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="250">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -1009,7 +1009,19 @@
     <t xml:space="preserve"> 2017-05-12 20:35:22</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve">2017-05-13-20:35:22 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        1.390 LTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            23.8 USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.185  USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LTC/USDT0000002</t>
   </si>
 </sst>
 </file>
@@ -1455,10 +1467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG56"/>
+  <dimension ref="A1:DG57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3407,7 +3419,7 @@
         <v>243</v>
       </c>
       <c r="E56" t="s">
-        <v>197</v>
+        <v>248</v>
       </c>
       <c r="F56" t="s">
         <v>242</v>
@@ -3416,13 +3428,43 @@
         <v>241</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="I56" s="6" t="s">
         <v>245</v>
       </c>
       <c r="K56" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>42871.274247685185</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" t="s">
+        <v>48</v>
+      </c>
+      <c r="D57">
+        <v>24.043316999999998</v>
+      </c>
+      <c r="E57" t="s">
+        <v>247</v>
+      </c>
+      <c r="F57" t="s">
+        <v>246</v>
+      </c>
+      <c r="G57" t="s">
+        <v>249</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I57" s="2"/>
+      <c r="K57" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated at 18.05.2017 in 20 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="259">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -1022,6 +1022,35 @@
   </si>
   <si>
     <t xml:space="preserve"> LTC/USDT0000002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            25 USDT</t>
+  </si>
+  <si>
+    <t>0.05704681 USDT (0.15%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ~5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.335  USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         111 XRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XRP/USDT0000007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              0.335
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.365  USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              0.333
+</t>
   </si>
 </sst>
 </file>
@@ -1467,10 +1496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG57"/>
+  <dimension ref="A1:DG60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3460,11 +3489,113 @@
         <v>249</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I57" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="I57" s="2">
+        <v>42871.3746875</v>
+      </c>
       <c r="K57" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>42871.3746875</v>
+      </c>
+      <c r="B58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" t="s">
+        <v>48</v>
+      </c>
+      <c r="D58">
+        <v>24.5</v>
+      </c>
+      <c r="E58" t="s">
+        <v>250</v>
+      </c>
+      <c r="F58" t="s">
+        <v>246</v>
+      </c>
+      <c r="G58" t="s">
+        <v>249</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I58" s="2">
+        <v>42872.466319444444</v>
+      </c>
+      <c r="J58" t="s">
+        <v>251</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="L58" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>42873.277673611112</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" t="s">
+        <v>107</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E59" t="s">
+        <v>253</v>
+      </c>
+      <c r="F59" t="s">
+        <v>254</v>
+      </c>
+      <c r="G59" t="s">
+        <v>255</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I59" s="6">
+        <v>42873.277673611112</v>
+      </c>
+      <c r="K59" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>42873.277673611112</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="E60" t="s">
+        <v>257</v>
+      </c>
+      <c r="F60" t="s">
+        <v>254</v>
+      </c>
+      <c r="G60" t="s">
+        <v>255</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I60" s="6"/>
+      <c r="K60" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated in 15 minutes
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="264">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -1051,6 +1051,34 @@
   <si>
     <t xml:space="preserve">              0.333
 </t>
+  </si>
+  <si>
+    <t>0.06062057 USDT (0.15%)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>~8.5%</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> XRP/USDT0000008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              0.37520001
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         121 XRP</t>
   </si>
 </sst>
 </file>
@@ -1496,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG60"/>
+  <dimension ref="A1:DG61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3591,10 +3619,48 @@
         <v>255</v>
       </c>
       <c r="H60" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I60" s="6">
+        <v>42873.451099537036</v>
+      </c>
+      <c r="J60" t="s">
+        <v>259</v>
+      </c>
+      <c r="K60" t="s">
+        <v>260</v>
+      </c>
+      <c r="L60" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>42873.451099537036</v>
+      </c>
+      <c r="B61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" t="s">
+        <v>107</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="E61" t="s">
+        <v>253</v>
+      </c>
+      <c r="F61" t="s">
+        <v>263</v>
+      </c>
+      <c r="G61" t="s">
+        <v>261</v>
+      </c>
+      <c r="H61" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I60" s="6"/>
-      <c r="K60" t="s">
+      <c r="I61" s="6"/>
+      <c r="K61" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated at 19.05.2017 in 15 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="268">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -1079,6 +1079,19 @@
   </si>
   <si>
     <t xml:space="preserve">         121 XRP</t>
+  </si>
+  <si>
+    <t>0.18150000 XRP (0.15%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         120 XRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.375  USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              0.337
+</t>
   </si>
 </sst>
 </file>
@@ -1524,10 +1537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG61"/>
+  <dimension ref="A1:DG62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3657,10 +3670,45 @@
         <v>261</v>
       </c>
       <c r="H61" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I61" s="6">
+        <v>42874.355543981481</v>
+      </c>
+      <c r="J61" t="s">
+        <v>264</v>
+      </c>
+      <c r="K61" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6">
+        <v>42874.355543981481</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" t="s">
+        <v>107</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E62" t="s">
+        <v>266</v>
+      </c>
+      <c r="F62" t="s">
+        <v>265</v>
+      </c>
+      <c r="G62" t="s">
+        <v>261</v>
+      </c>
+      <c r="H62" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I61" s="6"/>
-      <c r="K61" t="s">
+      <c r="I62" s="6"/>
+      <c r="K62" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated file at 20.05.2017 in 20 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="275">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -1087,11 +1087,45 @@
     <t xml:space="preserve">         120 XRP</t>
   </si>
   <si>
-    <t xml:space="preserve">         0.375  USDT</t>
-  </si>
-  <si>
     <t xml:space="preserve">              0.337
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.350  USDT</t>
+  </si>
+  <si>
+    <t>0.06342971 USDT (0.15%)</t>
+  </si>
+  <si>
+    <t>2.5 day</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>~4%</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.300  USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XRP/USDT0000009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              0.355
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         145 XRP</t>
   </si>
 </sst>
 </file>
@@ -1537,10 +1571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG62"/>
+  <dimension ref="A1:DG63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3693,10 +3727,10 @@
         <v>107</v>
       </c>
       <c r="D62" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="E62" t="s">
         <v>267</v>
-      </c>
-      <c r="E62" t="s">
-        <v>266</v>
       </c>
       <c r="F62" t="s">
         <v>265</v>
@@ -3705,10 +3739,48 @@
         <v>261</v>
       </c>
       <c r="H62" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I62" s="6">
+        <v>42875.454837962963</v>
+      </c>
+      <c r="J62" t="s">
+        <v>268</v>
+      </c>
+      <c r="K62" t="s">
+        <v>270</v>
+      </c>
+      <c r="L62" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>42875.451099537036</v>
+      </c>
+      <c r="B63" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" t="s">
+        <v>107</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="E63" t="s">
+        <v>271</v>
+      </c>
+      <c r="F63" t="s">
+        <v>274</v>
+      </c>
+      <c r="G63" t="s">
+        <v>272</v>
+      </c>
+      <c r="H63" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I62" s="6"/>
-      <c r="K62" t="s">
+      <c r="I63" s="6"/>
+      <c r="K63" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated file in 20 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="284">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -1126,6 +1126,45 @@
   </si>
   <si>
     <t xml:space="preserve">         145 XRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            26.4 USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        1.6 LTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            27.6 USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LTC/USDT0000003</t>
+  </si>
+  <si>
+    <t>0.06607440 USDT (0.15%)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ~4%</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.338  USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         134 XRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                5/21/2017  13:49:35 AM</t>
   </si>
 </sst>
 </file>
@@ -1571,10 +1610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG63"/>
+  <dimension ref="A1:DG66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3777,10 +3816,112 @@
         <v>272</v>
       </c>
       <c r="H63" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I63" s="6">
+        <v>42876.336493055554</v>
+      </c>
+      <c r="K63" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>42876.336493055554</v>
+      </c>
+      <c r="B64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" t="s">
+        <v>48</v>
+      </c>
+      <c r="D64">
+        <v>26.41</v>
+      </c>
+      <c r="E64" t="s">
+        <v>275</v>
+      </c>
+      <c r="F64" t="s">
+        <v>276</v>
+      </c>
+      <c r="G64" t="s">
+        <v>278</v>
+      </c>
+      <c r="H64" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I64" s="2">
+        <v>42876.336493055554</v>
+      </c>
+      <c r="K64" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>42876.336493055554</v>
+      </c>
+      <c r="B65" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" t="s">
+        <v>48</v>
+      </c>
+      <c r="D65">
+        <v>26.41</v>
+      </c>
+      <c r="E65" t="s">
+        <v>277</v>
+      </c>
+      <c r="F65" t="s">
+        <v>276</v>
+      </c>
+      <c r="G65" t="s">
+        <v>278</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I65" s="2">
+        <v>42876.504849537036</v>
+      </c>
+      <c r="J65" t="s">
+        <v>279</v>
+      </c>
+      <c r="K65" t="s">
+        <v>280</v>
+      </c>
+      <c r="L65" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="B66" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" t="s">
+        <v>107</v>
+      </c>
+      <c r="D66" s="7">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="E66" t="s">
+        <v>281</v>
+      </c>
+      <c r="F66" t="s">
+        <v>282</v>
+      </c>
+      <c r="G66" t="s">
+        <v>272</v>
+      </c>
+      <c r="H66" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I63" s="6"/>
-      <c r="K63" t="s">
+      <c r="I66" s="6"/>
+      <c r="K66" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated at 24.05.2017 in 20 min
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="298">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -1173,7 +1173,52 @@
     <t xml:space="preserve">                5/21/2017  14:49:35 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">         0.367  USDT</t>
+    <t xml:space="preserve">         0.340  USDT</t>
+  </si>
+  <si>
+    <t>0.06823749 USDT (0.15%)</t>
+  </si>
+  <si>
+    <t>2 day</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>~0.2%</t>
+    </r>
+  </si>
+  <si>
+    <t>0.21674578 XRP (0.15%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             2017-05-24 10:47:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.316  USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XRP/USDT0000010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                2017-05-24 10:47:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         144 XRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.342  USDT</t>
   </si>
 </sst>
 </file>
@@ -1619,10 +1664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG67"/>
+  <dimension ref="A1:DG69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3962,11 +4007,84 @@
         <v>272</v>
       </c>
       <c r="H67" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I67" s="6">
+        <v>42878.568287037036</v>
+      </c>
+      <c r="J67" t="s">
+        <v>287</v>
+      </c>
+      <c r="K67" t="s">
+        <v>289</v>
+      </c>
+      <c r="L67" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B68" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" t="s">
+        <v>107</v>
+      </c>
+      <c r="D68" s="7">
+        <v>0.3155</v>
+      </c>
+      <c r="E68" t="s">
+        <v>292</v>
+      </c>
+      <c r="F68" t="s">
+        <v>295</v>
+      </c>
+      <c r="G68" t="s">
+        <v>293</v>
+      </c>
+      <c r="H68" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I68" s="6">
+        <v>42879.449328703704</v>
+      </c>
+      <c r="J68" t="s">
+        <v>290</v>
+      </c>
+      <c r="K68" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="B69" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" t="s">
+        <v>107</v>
+      </c>
+      <c r="D69" s="7">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="E69" t="s">
+        <v>297</v>
+      </c>
+      <c r="F69" t="s">
+        <v>295</v>
+      </c>
+      <c r="G69" t="s">
+        <v>293</v>
+      </c>
+      <c r="H69" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I67" s="6"/>
-      <c r="K67" t="s">
-        <v>171</v>
+      <c r="I69" s="6"/>
+      <c r="K69" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added file with status at 23.10.2013
</commit_message>
<xml_diff>
--- a/poloniex history.xlsx
+++ b/poloniex history.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="338">
   <si>
     <t>Action(Buy/Sell)</t>
   </si>
@@ -1173,13 +1173,146 @@
     <t xml:space="preserve">                5/21/2017  14:49:35 AM</t>
   </si>
   <si>
+    <t xml:space="preserve"> XRP/USDT0000011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.208  USDT</t>
+  </si>
+  <si>
+    <t>9/12/2017  13:49:35 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                9/6/2017  13:49:35 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         460 XRP</t>
+  </si>
+  <si>
+    <t>0.69000000 XRP (0.15%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                9/13/2017  13:49:35 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.223  USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         459 XRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.15363920 USDT (0.15%) </t>
+  </si>
+  <si>
+    <t>~30</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>~7%</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> STR/USDT0000002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           0.01326502
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.0133 USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         7550 STR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.027 USDT</t>
+  </si>
+  <si>
+    <t>0.30531634 USDT (0.15%)</t>
+  </si>
+  <si>
+    <t>11 day</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STR/USDT0000003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.014 USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           0.0338
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         7500 STR</t>
+  </si>
+  <si>
+    <t>BCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        325.8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BCH/USDT0000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         306 USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.326 BCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.165  USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        610 XRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XRP/USDT0000012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             10/19/2017  12:00:00 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  10/23/2017  12:00:00 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             10/23/2017  12:00:00 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.186  USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        541 XRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ETC/USDT0000002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               10.07
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          9.6 USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        10.95 ETC</t>
+  </si>
+  <si>
     <t xml:space="preserve">         0.340  USDT</t>
   </si>
   <si>
     <t>0.06823749 USDT (0.15%)</t>
-  </si>
-  <si>
-    <t>2 day</t>
   </si>
   <si>
     <r>
@@ -1197,28 +1330,31 @@
     </r>
   </si>
   <si>
+    <t>2 day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             2017-05-24 10:47:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.316  USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         144 XRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XRP/USDT0000010</t>
+  </si>
+  <si>
     <t>0.21674578 XRP (0.15%)</t>
   </si>
   <si>
-    <t xml:space="preserve">             2017-05-24 10:47:02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         0.316  USDT</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> XRP/USDT0000010</t>
-  </si>
-  <si>
     <t xml:space="preserve">                2017-05-24 10:47:02</t>
   </si>
   <si>
-    <t xml:space="preserve">         144 XRP</t>
+    <t xml:space="preserve">         0.342  USDT</t>
   </si>
   <si>
     <t xml:space="preserve">    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">         0.342  USDT</t>
   </si>
 </sst>
 </file>
@@ -1316,7 +1452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1331,6 +1467,7 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1664,10 +1801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG69"/>
+  <dimension ref="A1:DG78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J76" sqref="J76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3980,9 +4117,7 @@
       <c r="J66" t="s">
         <v>284</v>
       </c>
-      <c r="K66" t="s">
-        <v>171</v>
-      </c>
+      <c r="K66" s="10"/>
     </row>
     <row r="67" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
@@ -3998,7 +4133,7 @@
         <v>0.33700000000000002</v>
       </c>
       <c r="E67" t="s">
-        <v>286</v>
+        <v>326</v>
       </c>
       <c r="F67" t="s">
         <v>282</v>
@@ -4013,18 +4148,18 @@
         <v>42878.568287037036</v>
       </c>
       <c r="J67" t="s">
-        <v>287</v>
+        <v>327</v>
       </c>
       <c r="K67" t="s">
-        <v>289</v>
+        <v>328</v>
       </c>
       <c r="L67" t="s">
-        <v>288</v>
+        <v>329</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>291</v>
+        <v>330</v>
       </c>
       <c r="B68" t="s">
         <v>11</v>
@@ -4036,13 +4171,13 @@
         <v>0.3155</v>
       </c>
       <c r="E68" t="s">
-        <v>292</v>
+        <v>331</v>
       </c>
       <c r="F68" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
       <c r="G68" t="s">
-        <v>293</v>
+        <v>333</v>
       </c>
       <c r="H68" s="9" t="s">
         <v>45</v>
@@ -4051,7 +4186,7 @@
         <v>42879.449328703704</v>
       </c>
       <c r="J68" t="s">
-        <v>290</v>
+        <v>334</v>
       </c>
       <c r="K68" t="s">
         <v>171</v>
@@ -4059,7 +4194,7 @@
     </row>
     <row r="69" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>294</v>
+        <v>335</v>
       </c>
       <c r="B69" t="s">
         <v>6</v>
@@ -4071,45 +4206,360 @@
         <v>0.31900000000000001</v>
       </c>
       <c r="E69" t="s">
-        <v>297</v>
+        <v>336</v>
       </c>
       <c r="F69" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
       <c r="G69" t="s">
-        <v>293</v>
+        <v>333</v>
       </c>
       <c r="H69" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I69" s="6"/>
       <c r="K69" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B70" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" t="s">
+        <v>107</v>
+      </c>
+      <c r="D70" s="7">
+        <v>0.222</v>
+      </c>
+      <c r="E70" t="s">
+        <v>287</v>
+      </c>
+      <c r="F70" t="s">
+        <v>290</v>
+      </c>
+      <c r="G70" t="s">
+        <v>286</v>
+      </c>
+      <c r="H70" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I70" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="J70" t="s">
+        <v>291</v>
+      </c>
+      <c r="K70" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="B71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" t="s">
+        <v>107</v>
+      </c>
+      <c r="D71" s="7">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="E71" t="s">
+        <v>293</v>
+      </c>
+      <c r="F71" t="s">
+        <v>294</v>
+      </c>
+      <c r="G71" t="s">
+        <v>286</v>
+      </c>
+      <c r="H71" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I71" s="6">
+        <v>43013</v>
+      </c>
+      <c r="J71" t="s">
+        <v>295</v>
+      </c>
+      <c r="K71" t="s">
+        <v>297</v>
+      </c>
+      <c r="L71" t="s">
         <v>296</v>
       </c>
+    </row>
+    <row r="72" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="6">
+        <v>43013</v>
+      </c>
+      <c r="B72" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" t="s">
+        <v>209</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="E72" t="s">
+        <v>300</v>
+      </c>
+      <c r="F72" t="s">
+        <v>301</v>
+      </c>
+      <c r="G72" t="s">
+        <v>298</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I72" s="6">
+        <v>43013</v>
+      </c>
+      <c r="J72" t="s">
+        <v>214</v>
+      </c>
+      <c r="K72" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="6">
+        <v>43013</v>
+      </c>
+      <c r="B73" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" t="s">
+        <v>209</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="E73" t="s">
+        <v>302</v>
+      </c>
+      <c r="F73" t="s">
+        <v>301</v>
+      </c>
+      <c r="G73" t="s">
+        <v>298</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I73" s="6">
+        <v>43024.259664351855</v>
+      </c>
+      <c r="J73" t="s">
+        <v>303</v>
+      </c>
+      <c r="K73" s="10">
+        <v>2</v>
+      </c>
+      <c r="L73" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="6">
+        <v>43026</v>
+      </c>
+      <c r="B74" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" t="s">
+        <v>209</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="E74" t="s">
+        <v>306</v>
+      </c>
+      <c r="F74" t="s">
+        <v>308</v>
+      </c>
+      <c r="G74" t="s">
+        <v>305</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I74" s="6"/>
+      <c r="K74" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="6">
+        <v>43026</v>
+      </c>
+      <c r="B75" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" t="s">
+        <v>223</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="E75" t="s">
+        <v>312</v>
+      </c>
+      <c r="F75" t="s">
+        <v>313</v>
+      </c>
+      <c r="G75" t="s">
+        <v>311</v>
+      </c>
+      <c r="H75" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I75" s="6">
+        <v>43027</v>
+      </c>
+      <c r="K75" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="B76" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" t="s">
+        <v>107</v>
+      </c>
+      <c r="D76" s="7">
+        <v>0.216</v>
+      </c>
+      <c r="E76" t="s">
+        <v>314</v>
+      </c>
+      <c r="F76" t="s">
+        <v>315</v>
+      </c>
+      <c r="G76" t="s">
+        <v>316</v>
+      </c>
+      <c r="H76" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I76" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="K76" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="B77" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" t="s">
+        <v>107</v>
+      </c>
+      <c r="D77" s="7">
+        <v>0.189</v>
+      </c>
+      <c r="E77" t="s">
+        <v>320</v>
+      </c>
+      <c r="F77" t="s">
+        <v>321</v>
+      </c>
+      <c r="G77" t="s">
+        <v>316</v>
+      </c>
+      <c r="H77" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I77" s="6"/>
+      <c r="K77" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="6">
+        <v>43031.441886574074</v>
+      </c>
+      <c r="B78" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" t="s">
+        <v>58</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="E78" t="s">
+        <v>324</v>
+      </c>
+      <c r="F78" t="s">
+        <v>325</v>
+      </c>
+      <c r="G78" t="s">
+        <v>322</v>
+      </c>
+      <c r="H78" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I78" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
+          <xm:sqref>H1:H66 H70:H1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C1048576</xm:sqref>
+          <xm:sqref>C1:C66 C70:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$C$1:$C$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:B1048576</xm:sqref>
+          <xm:sqref>B1:B66 B70:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Sheet2!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>B67:B69</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Sheet2!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>C67:C69</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Sheet2!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>H67:H69</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4119,10 +4569,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4207,6 +4657,11 @@
         <v>233</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>309</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>